<commit_message>
modificacion nombre en leads
</commit_message>
<xml_diff>
--- a/public/temp/PlantillaLeads.xlsx
+++ b/public/temp/PlantillaLeads.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159D28E7-8DEA-4A0F-8D10-7A9A245D69A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52CE531-FF40-4D49-A85B-14B5EB083988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -543,9 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1582,9 +1579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC508"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1611,7 +1606,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="8" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
@@ -1626,7 +1621,7 @@
       <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="8" t="s">
         <v>118</v>
       </c>
       <c r="G1" s="9" t="s">
@@ -1692,7 +1687,7 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
-      <c r="F2" s="17"/>
+      <c r="F2" s="16"/>
       <c r="I2" s="12"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
@@ -1701,7 +1696,7 @@
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
       <c r="I3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
@@ -1714,21 +1709,21 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B4" s="7"/>
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
       <c r="I4" s="12"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B5" s="7"/>
-      <c r="F5" s="17"/>
+      <c r="F5" s="16"/>
       <c r="I5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B6" s="7"/>
-      <c r="F6" s="17"/>
+      <c r="F6" s="16"/>
       <c r="I6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
@@ -1736,896 +1731,896 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B7" s="7"/>
-      <c r="F7" s="17"/>
+      <c r="F7" s="16"/>
       <c r="I7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B8" s="7"/>
-      <c r="F8" s="17"/>
+      <c r="F8" s="16"/>
       <c r="I8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B9" s="7"/>
-      <c r="F9" s="17"/>
+      <c r="F9" s="16"/>
       <c r="I9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B10" s="7"/>
-      <c r="F10" s="17"/>
+      <c r="F10" s="16"/>
       <c r="I10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
-      <c r="F11" s="17"/>
+      <c r="F11" s="16"/>
       <c r="I11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
-      <c r="F12" s="17"/>
+      <c r="F12" s="16"/>
       <c r="I12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B13" s="7"/>
-      <c r="F13" s="17"/>
+      <c r="F13" s="16"/>
       <c r="I13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B14" s="7"/>
-      <c r="F14" s="17"/>
+      <c r="F14" s="16"/>
       <c r="I14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B15" s="7"/>
-      <c r="F15" s="17"/>
+      <c r="F15" s="16"/>
       <c r="I15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="B16" s="7"/>
-      <c r="F16" s="17"/>
+      <c r="F16" s="16"/>
       <c r="I16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B17" s="7"/>
-      <c r="F17" s="17"/>
+      <c r="F17" s="16"/>
       <c r="I17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B18" s="7"/>
-      <c r="F18" s="17"/>
+      <c r="F18" s="16"/>
       <c r="I18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B19" s="7"/>
-      <c r="F19" s="17"/>
+      <c r="F19" s="16"/>
       <c r="I19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B20" s="7"/>
-      <c r="F20" s="17"/>
+      <c r="F20" s="16"/>
       <c r="I20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B21" s="7"/>
-      <c r="F21" s="17"/>
+      <c r="F21" s="16"/>
       <c r="I21" s="12"/>
       <c r="L21" s="12"/>
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B22" s="7"/>
-      <c r="F22" s="17"/>
+      <c r="F22" s="16"/>
       <c r="I22" s="12"/>
       <c r="L22" s="12"/>
       <c r="M22" s="12"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B23" s="7"/>
-      <c r="F23" s="17"/>
+      <c r="F23" s="16"/>
       <c r="I23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B24" s="7"/>
-      <c r="F24" s="17"/>
+      <c r="F24" s="16"/>
       <c r="I24" s="12"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B25" s="7"/>
-      <c r="F25" s="17"/>
+      <c r="F25" s="16"/>
       <c r="I25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B26" s="7"/>
-      <c r="F26" s="17"/>
+      <c r="F26" s="16"/>
       <c r="I26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B27" s="7"/>
-      <c r="F27" s="17"/>
+      <c r="F27" s="16"/>
       <c r="I27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B28" s="7"/>
-      <c r="F28" s="17"/>
+      <c r="F28" s="16"/>
       <c r="I28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B29" s="7"/>
-      <c r="F29" s="17"/>
+      <c r="F29" s="16"/>
       <c r="I29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B30" s="7"/>
-      <c r="F30" s="17"/>
+      <c r="F30" s="16"/>
       <c r="I30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B31" s="7"/>
-      <c r="F31" s="17"/>
+      <c r="F31" s="16"/>
       <c r="I31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B32" s="7"/>
-      <c r="F32" s="17"/>
+      <c r="F32" s="16"/>
       <c r="I32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
     </row>
     <row r="33" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B33" s="7"/>
-      <c r="F33" s="17"/>
+      <c r="F33" s="16"/>
       <c r="I33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B34" s="7"/>
-      <c r="F34" s="17"/>
+      <c r="F34" s="16"/>
       <c r="I34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B35" s="7"/>
-      <c r="F35" s="17"/>
+      <c r="F35" s="16"/>
       <c r="I35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
     </row>
     <row r="36" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B36" s="7"/>
-      <c r="F36" s="17"/>
+      <c r="F36" s="16"/>
       <c r="I36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B37" s="7"/>
-      <c r="F37" s="17"/>
+      <c r="F37" s="16"/>
       <c r="I37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
     </row>
     <row r="38" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B38" s="7"/>
-      <c r="F38" s="17"/>
+      <c r="F38" s="16"/>
       <c r="I38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
     </row>
     <row r="39" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B39" s="7"/>
-      <c r="F39" s="17"/>
+      <c r="F39" s="16"/>
       <c r="I39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B40" s="7"/>
-      <c r="F40" s="17"/>
+      <c r="F40" s="16"/>
       <c r="I40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B41" s="7"/>
-      <c r="F41" s="17"/>
+      <c r="F41" s="16"/>
       <c r="I41" s="12"/>
       <c r="L41" s="12"/>
       <c r="M41" s="12"/>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B42" s="7"/>
-      <c r="F42" s="17"/>
+      <c r="F42" s="16"/>
       <c r="I42" s="12"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B43" s="7"/>
-      <c r="F43" s="17"/>
+      <c r="F43" s="16"/>
       <c r="I43" s="12"/>
       <c r="L43" s="12"/>
       <c r="M43" s="12"/>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B44" s="7"/>
-      <c r="F44" s="17"/>
+      <c r="F44" s="16"/>
       <c r="I44" s="12"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B45" s="7"/>
-      <c r="F45" s="17"/>
+      <c r="F45" s="16"/>
       <c r="I45" s="12"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B46" s="7"/>
-      <c r="F46" s="17"/>
+      <c r="F46" s="16"/>
       <c r="I46" s="12"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B47" s="7"/>
-      <c r="F47" s="17"/>
+      <c r="F47" s="16"/>
       <c r="I47" s="12"/>
       <c r="L47" s="12"/>
       <c r="M47" s="12"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B48" s="7"/>
-      <c r="F48" s="17"/>
+      <c r="F48" s="16"/>
       <c r="I48" s="12"/>
       <c r="L48" s="12"/>
       <c r="M48" s="12"/>
     </row>
     <row r="49" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B49" s="7"/>
-      <c r="F49" s="17"/>
+      <c r="F49" s="16"/>
       <c r="I49" s="12"/>
       <c r="L49" s="12"/>
       <c r="M49" s="12"/>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B50" s="7"/>
-      <c r="F50" s="17"/>
+      <c r="F50" s="16"/>
       <c r="I50" s="12"/>
       <c r="L50" s="12"/>
       <c r="M50" s="12"/>
     </row>
     <row r="51" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B51" s="7"/>
-      <c r="F51" s="17"/>
+      <c r="F51" s="16"/>
       <c r="I51" s="12"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B52" s="7"/>
-      <c r="F52" s="17"/>
+      <c r="F52" s="16"/>
       <c r="I52" s="12"/>
       <c r="L52" s="12"/>
       <c r="M52" s="12"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B53" s="7"/>
-      <c r="F53" s="17"/>
+      <c r="F53" s="16"/>
       <c r="I53" s="12"/>
       <c r="L53" s="12"/>
       <c r="M53" s="12"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B54" s="7"/>
-      <c r="F54" s="17"/>
+      <c r="F54" s="16"/>
       <c r="I54" s="12"/>
       <c r="L54" s="12"/>
       <c r="M54" s="12"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B55" s="7"/>
-      <c r="F55" s="17"/>
+      <c r="F55" s="16"/>
       <c r="I55" s="12"/>
       <c r="L55" s="12"/>
       <c r="M55" s="12"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B56" s="7"/>
-      <c r="F56" s="17"/>
+      <c r="F56" s="16"/>
       <c r="I56" s="12"/>
       <c r="L56" s="12"/>
       <c r="M56" s="12"/>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B57" s="7"/>
-      <c r="F57" s="17"/>
+      <c r="F57" s="16"/>
       <c r="I57" s="12"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
     </row>
     <row r="58" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B58" s="7"/>
-      <c r="F58" s="17"/>
+      <c r="F58" s="16"/>
       <c r="I58" s="12"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
     </row>
     <row r="59" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B59" s="7"/>
-      <c r="F59" s="17"/>
+      <c r="F59" s="16"/>
       <c r="I59" s="12"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12"/>
     </row>
     <row r="60" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B60" s="7"/>
-      <c r="F60" s="17"/>
+      <c r="F60" s="16"/>
       <c r="I60" s="12"/>
       <c r="L60" s="12"/>
       <c r="M60" s="12"/>
     </row>
     <row r="61" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B61" s="7"/>
-      <c r="F61" s="17"/>
+      <c r="F61" s="16"/>
       <c r="I61" s="12"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
     </row>
     <row r="62" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B62" s="7"/>
-      <c r="F62" s="17"/>
+      <c r="F62" s="16"/>
       <c r="I62" s="12"/>
       <c r="L62" s="12"/>
       <c r="M62" s="12"/>
     </row>
     <row r="63" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B63" s="7"/>
-      <c r="F63" s="17"/>
+      <c r="F63" s="16"/>
       <c r="I63" s="12"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
     </row>
     <row r="64" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B64" s="7"/>
-      <c r="F64" s="17"/>
+      <c r="F64" s="16"/>
       <c r="I64" s="12"/>
       <c r="L64" s="12"/>
       <c r="M64" s="12"/>
     </row>
     <row r="65" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B65" s="7"/>
-      <c r="F65" s="17"/>
+      <c r="F65" s="16"/>
       <c r="I65" s="12"/>
       <c r="L65" s="12"/>
       <c r="M65" s="12"/>
     </row>
     <row r="66" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B66" s="7"/>
-      <c r="F66" s="17"/>
+      <c r="F66" s="16"/>
       <c r="I66" s="12"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
     </row>
     <row r="67" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B67" s="7"/>
-      <c r="F67" s="17"/>
+      <c r="F67" s="16"/>
       <c r="I67" s="12"/>
       <c r="L67" s="12"/>
       <c r="M67" s="12"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B68" s="7"/>
-      <c r="F68" s="17"/>
+      <c r="F68" s="16"/>
       <c r="I68" s="12"/>
       <c r="L68" s="12"/>
       <c r="M68" s="12"/>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B69" s="7"/>
-      <c r="F69" s="17"/>
+      <c r="F69" s="16"/>
       <c r="I69" s="12"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12"/>
     </row>
     <row r="70" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B70" s="7"/>
-      <c r="F70" s="17"/>
+      <c r="F70" s="16"/>
       <c r="I70" s="12"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12"/>
     </row>
     <row r="71" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B71" s="7"/>
-      <c r="F71" s="17"/>
+      <c r="F71" s="16"/>
       <c r="I71" s="12"/>
       <c r="L71" s="12"/>
       <c r="M71" s="12"/>
     </row>
     <row r="72" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B72" s="7"/>
-      <c r="F72" s="17"/>
+      <c r="F72" s="16"/>
       <c r="I72" s="12"/>
       <c r="L72" s="12"/>
       <c r="M72" s="12"/>
     </row>
     <row r="73" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B73" s="7"/>
-      <c r="F73" s="17"/>
+      <c r="F73" s="16"/>
       <c r="I73" s="12"/>
       <c r="L73" s="12"/>
       <c r="M73" s="12"/>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B74" s="7"/>
-      <c r="F74" s="17"/>
+      <c r="F74" s="16"/>
       <c r="I74" s="12"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12"/>
     </row>
     <row r="75" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B75" s="7"/>
-      <c r="F75" s="17"/>
+      <c r="F75" s="16"/>
       <c r="I75" s="12"/>
       <c r="L75" s="12"/>
       <c r="M75" s="12"/>
     </row>
     <row r="76" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B76" s="7"/>
-      <c r="F76" s="17"/>
+      <c r="F76" s="16"/>
       <c r="I76" s="12"/>
       <c r="L76" s="12"/>
       <c r="M76" s="12"/>
     </row>
     <row r="77" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B77" s="7"/>
-      <c r="F77" s="17"/>
+      <c r="F77" s="16"/>
       <c r="I77" s="12"/>
       <c r="L77" s="12"/>
       <c r="M77" s="12"/>
     </row>
     <row r="78" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B78" s="7"/>
-      <c r="F78" s="17"/>
+      <c r="F78" s="16"/>
       <c r="I78" s="12"/>
       <c r="L78" s="12"/>
       <c r="M78" s="12"/>
     </row>
     <row r="79" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B79" s="7"/>
-      <c r="F79" s="17"/>
+      <c r="F79" s="16"/>
       <c r="I79" s="12"/>
       <c r="L79" s="12"/>
       <c r="M79" s="12"/>
     </row>
     <row r="80" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B80" s="7"/>
-      <c r="F80" s="17"/>
+      <c r="F80" s="16"/>
       <c r="I80" s="12"/>
       <c r="L80" s="12"/>
       <c r="M80" s="12"/>
     </row>
     <row r="81" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B81" s="7"/>
-      <c r="F81" s="17"/>
+      <c r="F81" s="16"/>
       <c r="I81" s="12"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
     </row>
     <row r="82" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B82" s="7"/>
-      <c r="F82" s="17"/>
+      <c r="F82" s="16"/>
       <c r="I82" s="12"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B83" s="7"/>
-      <c r="F83" s="17"/>
+      <c r="F83" s="16"/>
       <c r="I83" s="12"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
     </row>
     <row r="84" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B84" s="7"/>
-      <c r="F84" s="17"/>
+      <c r="F84" s="16"/>
       <c r="I84" s="12"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
     </row>
     <row r="85" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B85" s="7"/>
-      <c r="F85" s="17"/>
+      <c r="F85" s="16"/>
       <c r="I85" s="12"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
     </row>
     <row r="86" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B86" s="7"/>
-      <c r="F86" s="17"/>
+      <c r="F86" s="16"/>
       <c r="I86" s="12"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
     </row>
     <row r="87" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B87" s="7"/>
-      <c r="F87" s="17"/>
+      <c r="F87" s="16"/>
       <c r="I87" s="12"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B88" s="7"/>
-      <c r="F88" s="17"/>
+      <c r="F88" s="16"/>
       <c r="I88" s="12"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
     </row>
     <row r="89" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B89" s="7"/>
-      <c r="F89" s="17"/>
+      <c r="F89" s="16"/>
       <c r="I89" s="12"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
     </row>
     <row r="90" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B90" s="7"/>
-      <c r="F90" s="17"/>
+      <c r="F90" s="16"/>
       <c r="I90" s="12"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
     </row>
     <row r="91" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B91" s="7"/>
-      <c r="F91" s="17"/>
+      <c r="F91" s="16"/>
       <c r="I91" s="12"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
     </row>
     <row r="92" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B92" s="7"/>
-      <c r="F92" s="17"/>
+      <c r="F92" s="16"/>
       <c r="I92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
     </row>
     <row r="93" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B93" s="7"/>
-      <c r="F93" s="17"/>
+      <c r="F93" s="16"/>
       <c r="I93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
     </row>
     <row r="94" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B94" s="7"/>
-      <c r="F94" s="17"/>
+      <c r="F94" s="16"/>
       <c r="I94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
     </row>
     <row r="95" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B95" s="7"/>
-      <c r="F95" s="17"/>
+      <c r="F95" s="16"/>
       <c r="I95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
     </row>
     <row r="96" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B96" s="7"/>
-      <c r="F96" s="17"/>
+      <c r="F96" s="16"/>
       <c r="I96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
     </row>
     <row r="97" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B97" s="7"/>
-      <c r="F97" s="17"/>
+      <c r="F97" s="16"/>
       <c r="I97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
     </row>
     <row r="98" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B98" s="7"/>
-      <c r="F98" s="17"/>
+      <c r="F98" s="16"/>
       <c r="I98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12"/>
     </row>
     <row r="99" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B99" s="7"/>
-      <c r="F99" s="17"/>
+      <c r="F99" s="16"/>
       <c r="I99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12"/>
     </row>
     <row r="100" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B100" s="7"/>
-      <c r="F100" s="17"/>
+      <c r="F100" s="16"/>
       <c r="I100" s="12"/>
       <c r="L100" s="12"/>
       <c r="M100" s="12"/>
     </row>
     <row r="101" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B101" s="7"/>
-      <c r="F101" s="17"/>
+      <c r="F101" s="16"/>
       <c r="I101" s="12"/>
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
     </row>
     <row r="102" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B102" s="7"/>
-      <c r="F102" s="17"/>
+      <c r="F102" s="16"/>
       <c r="I102" s="12"/>
       <c r="L102" s="12"/>
       <c r="M102" s="12"/>
     </row>
     <row r="103" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B103" s="7"/>
-      <c r="F103" s="17"/>
+      <c r="F103" s="16"/>
       <c r="I103" s="12"/>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
     </row>
     <row r="104" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B104" s="7"/>
-      <c r="F104" s="17"/>
+      <c r="F104" s="16"/>
       <c r="I104" s="12"/>
       <c r="L104" s="12"/>
       <c r="M104" s="12"/>
     </row>
     <row r="105" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B105" s="7"/>
-      <c r="F105" s="17"/>
+      <c r="F105" s="16"/>
       <c r="I105" s="12"/>
       <c r="L105" s="12"/>
       <c r="M105" s="12"/>
     </row>
     <row r="106" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B106" s="7"/>
-      <c r="F106" s="17"/>
+      <c r="F106" s="16"/>
       <c r="I106" s="12"/>
       <c r="L106" s="12"/>
       <c r="M106" s="12"/>
     </row>
     <row r="107" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B107" s="7"/>
-      <c r="F107" s="17"/>
+      <c r="F107" s="16"/>
       <c r="I107" s="12"/>
       <c r="L107" s="12"/>
       <c r="M107" s="12"/>
     </row>
     <row r="108" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B108" s="7"/>
-      <c r="F108" s="17"/>
+      <c r="F108" s="16"/>
       <c r="I108" s="12"/>
       <c r="L108" s="12"/>
       <c r="M108" s="12"/>
     </row>
     <row r="109" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B109" s="7"/>
-      <c r="F109" s="17"/>
+      <c r="F109" s="16"/>
       <c r="I109" s="12"/>
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
     </row>
     <row r="110" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B110" s="7"/>
-      <c r="F110" s="17"/>
+      <c r="F110" s="16"/>
       <c r="I110" s="12"/>
       <c r="L110" s="12"/>
       <c r="M110" s="12"/>
     </row>
     <row r="111" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B111" s="7"/>
-      <c r="F111" s="17"/>
+      <c r="F111" s="16"/>
       <c r="I111" s="12"/>
       <c r="L111" s="12"/>
       <c r="M111" s="12"/>
     </row>
     <row r="112" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B112" s="7"/>
-      <c r="F112" s="17"/>
+      <c r="F112" s="16"/>
       <c r="I112" s="12"/>
       <c r="L112" s="12"/>
       <c r="M112" s="12"/>
     </row>
     <row r="113" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B113" s="7"/>
-      <c r="F113" s="17"/>
+      <c r="F113" s="16"/>
       <c r="I113" s="12"/>
       <c r="L113" s="12"/>
       <c r="M113" s="12"/>
     </row>
     <row r="114" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B114" s="7"/>
-      <c r="F114" s="17"/>
+      <c r="F114" s="16"/>
       <c r="I114" s="12"/>
       <c r="L114" s="12"/>
       <c r="M114" s="12"/>
     </row>
     <row r="115" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B115" s="7"/>
-      <c r="F115" s="17"/>
+      <c r="F115" s="16"/>
       <c r="I115" s="12"/>
       <c r="L115" s="12"/>
       <c r="M115" s="12"/>
     </row>
     <row r="116" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B116" s="7"/>
-      <c r="F116" s="17"/>
+      <c r="F116" s="16"/>
       <c r="I116" s="12"/>
       <c r="L116" s="12"/>
       <c r="M116" s="12"/>
     </row>
     <row r="117" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B117" s="7"/>
-      <c r="F117" s="17"/>
+      <c r="F117" s="16"/>
       <c r="I117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
     </row>
     <row r="118" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B118" s="7"/>
-      <c r="F118" s="17"/>
+      <c r="F118" s="16"/>
       <c r="I118" s="12"/>
       <c r="L118" s="12"/>
       <c r="M118" s="12"/>
     </row>
     <row r="119" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B119" s="7"/>
-      <c r="F119" s="17"/>
+      <c r="F119" s="16"/>
       <c r="I119" s="12"/>
       <c r="L119" s="12"/>
       <c r="M119" s="12"/>
     </row>
     <row r="120" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B120" s="7"/>
-      <c r="F120" s="17"/>
+      <c r="F120" s="16"/>
       <c r="I120" s="12"/>
       <c r="L120" s="12"/>
       <c r="M120" s="12"/>
     </row>
     <row r="121" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B121" s="7"/>
-      <c r="F121" s="17"/>
+      <c r="F121" s="16"/>
       <c r="I121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
     </row>
     <row r="122" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B122" s="7"/>
-      <c r="F122" s="17"/>
+      <c r="F122" s="16"/>
       <c r="I122" s="12"/>
       <c r="L122" s="12"/>
       <c r="M122" s="12"/>
     </row>
     <row r="123" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B123" s="7"/>
-      <c r="F123" s="17"/>
+      <c r="F123" s="16"/>
       <c r="I123" s="12"/>
       <c r="L123" s="12"/>
       <c r="M123" s="12"/>
     </row>
     <row r="124" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B124" s="7"/>
-      <c r="F124" s="17"/>
+      <c r="F124" s="16"/>
       <c r="I124" s="12"/>
       <c r="L124" s="12"/>
       <c r="M124" s="12"/>
     </row>
     <row r="125" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B125" s="7"/>
-      <c r="F125" s="17"/>
+      <c r="F125" s="16"/>
       <c r="I125" s="12"/>
       <c r="L125" s="12"/>
       <c r="M125" s="12"/>
     </row>
     <row r="126" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B126" s="7"/>
-      <c r="F126" s="17"/>
+      <c r="F126" s="16"/>
       <c r="I126" s="12"/>
       <c r="L126" s="12"/>
       <c r="M126" s="12"/>
     </row>
     <row r="127" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B127" s="7"/>
-      <c r="F127" s="17"/>
+      <c r="F127" s="16"/>
       <c r="I127" s="12"/>
       <c r="L127" s="12"/>
       <c r="M127" s="12"/>
     </row>
     <row r="128" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B128" s="7"/>
-      <c r="F128" s="17"/>
+      <c r="F128" s="16"/>
       <c r="I128" s="12"/>
       <c r="L128" s="12"/>
       <c r="M128" s="12"/>
     </row>
     <row r="129" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B129" s="7"/>
-      <c r="F129" s="17"/>
+      <c r="F129" s="16"/>
       <c r="I129" s="12"/>
       <c r="L129" s="12"/>
       <c r="M129" s="12"/>
     </row>
     <row r="130" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B130" s="7"/>
-      <c r="F130" s="17"/>
+      <c r="F130" s="16"/>
       <c r="I130" s="12"/>
       <c r="L130" s="12"/>
       <c r="M130" s="12"/>
     </row>
     <row r="131" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B131" s="7"/>
-      <c r="F131" s="17"/>
+      <c r="F131" s="16"/>
       <c r="I131" s="12"/>
       <c r="L131" s="12"/>
       <c r="M131" s="12"/>
     </row>
     <row r="132" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B132" s="7"/>
-      <c r="F132" s="17"/>
+      <c r="F132" s="16"/>
       <c r="I132" s="12"/>
       <c r="L132" s="12"/>
       <c r="M132" s="12"/>
     </row>
     <row r="133" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B133" s="7"/>
-      <c r="F133" s="17"/>
+      <c r="F133" s="16"/>
       <c r="I133" s="12"/>
       <c r="L133" s="12"/>
       <c r="M133" s="12"/>
     </row>
     <row r="134" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B134" s="7"/>
-      <c r="F134" s="17"/>
+      <c r="F134" s="16"/>
       <c r="I134" s="12"/>
       <c r="L134" s="12"/>
       <c r="M134" s="12"/>

</xml_diff>